<commit_message>
feat: Inclusion of columns in the final version of the data frame
</commit_message>
<xml_diff>
--- a/GeoDados_flags.xlsx
+++ b/GeoDados_flags.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E251"/>
+  <dimension ref="A1:G251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,16 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Area em km2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>População</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>URL Bandeira</t>
         </is>
       </c>
@@ -481,7 +491,13 @@
           <t>Andorra la Vella</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" t="n">
+        <v>468</v>
+      </c>
+      <c r="F2" t="n">
+        <v>77006</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ad.gif</t>
         </is>
@@ -508,7 +524,13 @@
           <t>Abu Dhabi</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" t="n">
+        <v>82880</v>
+      </c>
+      <c r="F3" t="n">
+        <v>9630959</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ae.gif</t>
         </is>
@@ -535,7 +557,13 @@
           <t>Kabul</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" t="n">
+        <v>647500</v>
+      </c>
+      <c r="F4" t="n">
+        <v>37172386</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/af.gif</t>
         </is>
@@ -562,7 +590,13 @@
           <t>St. John's</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" t="n">
+        <v>443</v>
+      </c>
+      <c r="F5" t="n">
+        <v>96286</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ag.gif</t>
         </is>
@@ -589,7 +623,13 @@
           <t>The Valley</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" t="n">
+        <v>102</v>
+      </c>
+      <c r="F6" t="n">
+        <v>13254</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ai.gif</t>
         </is>
@@ -616,7 +656,13 @@
           <t>Tirana</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" t="n">
+        <v>28748</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2866376</v>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/al.gif</t>
         </is>
@@ -643,7 +689,13 @@
           <t>Yerevan</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" t="n">
+        <v>29800</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2951776</v>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/am.gif</t>
         </is>
@@ -670,7 +722,13 @@
           <t>Luanda</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" t="n">
+        <v>1246700</v>
+      </c>
+      <c r="F9" t="n">
+        <v>30809762</v>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ao.gif</t>
         </is>
@@ -697,7 +755,13 @@
           <t>Antártica</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" t="n">
+        <v>14000000</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/aq.gif</t>
         </is>
@@ -724,7 +788,13 @@
           <t>Buenos Aires</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" t="n">
+        <v>2766890</v>
+      </c>
+      <c r="F11" t="n">
+        <v>44494502</v>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ar.gif</t>
         </is>
@@ -751,7 +821,13 @@
           <t>Pago Pago</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" t="n">
+        <v>199</v>
+      </c>
+      <c r="F12" t="n">
+        <v>55465</v>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/as.gif</t>
         </is>
@@ -778,7 +854,13 @@
           <t>Vienna</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E13" t="n">
+        <v>83858</v>
+      </c>
+      <c r="F13" t="n">
+        <v>8847037</v>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/at.gif</t>
         </is>
@@ -805,7 +887,13 @@
           <t>Canberra</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" t="n">
+        <v>7686850</v>
+      </c>
+      <c r="F14" t="n">
+        <v>24992369</v>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/au.gif</t>
         </is>
@@ -832,7 +920,13 @@
           <t>Oranjestad</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" t="n">
+        <v>193</v>
+      </c>
+      <c r="F15" t="n">
+        <v>105845</v>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/aw.gif</t>
         </is>
@@ -859,7 +953,13 @@
           <t>Mariehamn</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E16" t="n">
+        <v>1580</v>
+      </c>
+      <c r="F16" t="n">
+        <v>26711</v>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ax.gif</t>
         </is>
@@ -886,7 +986,13 @@
           <t>Baku</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E17" t="n">
+        <v>86600</v>
+      </c>
+      <c r="F17" t="n">
+        <v>9942334</v>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/az.gif</t>
         </is>
@@ -913,7 +1019,13 @@
           <t>Sarajevo</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E18" t="n">
+        <v>51129</v>
+      </c>
+      <c r="F18" t="n">
+        <v>3323929</v>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ba.gif</t>
         </is>
@@ -940,7 +1052,13 @@
           <t>Bridgetown</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E19" t="n">
+        <v>431</v>
+      </c>
+      <c r="F19" t="n">
+        <v>286641</v>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bb.gif</t>
         </is>
@@ -967,7 +1085,13 @@
           <t>Dhaka</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E20" t="n">
+        <v>144000</v>
+      </c>
+      <c r="F20" t="n">
+        <v>161356039</v>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bd.gif</t>
         </is>
@@ -994,7 +1118,13 @@
           <t>Brussels</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="E21" t="n">
+        <v>30510</v>
+      </c>
+      <c r="F21" t="n">
+        <v>11422068</v>
+      </c>
+      <c r="G21" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/be.gif</t>
         </is>
@@ -1021,7 +1151,13 @@
           <t>Ouagadougou</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E22" t="n">
+        <v>274200</v>
+      </c>
+      <c r="F22" t="n">
+        <v>19751535</v>
+      </c>
+      <c r="G22" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bf.gif</t>
         </is>
@@ -1048,7 +1184,13 @@
           <t>Sofia</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E23" t="n">
+        <v>110910</v>
+      </c>
+      <c r="F23" t="n">
+        <v>7000039</v>
+      </c>
+      <c r="G23" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bg.gif</t>
         </is>
@@ -1075,7 +1217,13 @@
           <t>Manama</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="E24" t="n">
+        <v>665</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1569439</v>
+      </c>
+      <c r="G24" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bh.gif</t>
         </is>
@@ -1102,7 +1250,13 @@
           <t>Gitega</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="E25" t="n">
+        <v>27830</v>
+      </c>
+      <c r="F25" t="n">
+        <v>11175378</v>
+      </c>
+      <c r="G25" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bi.gif</t>
         </is>
@@ -1129,7 +1283,13 @@
           <t>Porto-Novo</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="E26" t="n">
+        <v>112620</v>
+      </c>
+      <c r="F26" t="n">
+        <v>11485048</v>
+      </c>
+      <c r="G26" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bj.gif</t>
         </is>
@@ -1156,7 +1316,13 @@
           <t>Gustavia</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="E27" t="n">
+        <v>21</v>
+      </c>
+      <c r="F27" t="n">
+        <v>8450</v>
+      </c>
+      <c r="G27" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bl.gif</t>
         </is>
@@ -1183,7 +1349,13 @@
           <t>Hamilton</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E28" t="n">
+        <v>53</v>
+      </c>
+      <c r="F28" t="n">
+        <v>63968</v>
+      </c>
+      <c r="G28" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bm.gif</t>
         </is>
@@ -1210,7 +1382,13 @@
           <t>Bandar Seri Begawan</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="E29" t="n">
+        <v>5770</v>
+      </c>
+      <c r="F29" t="n">
+        <v>428962</v>
+      </c>
+      <c r="G29" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bn.gif</t>
         </is>
@@ -1237,7 +1415,13 @@
           <t>Sucre</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="E30" t="n">
+        <v>1098580</v>
+      </c>
+      <c r="F30" t="n">
+        <v>11353142</v>
+      </c>
+      <c r="G30" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bo.gif</t>
         </is>
@@ -1264,7 +1448,13 @@
           <t>Bonaire, Santo Eustáquio e Saba</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E31" t="n">
+        <v>328</v>
+      </c>
+      <c r="F31" t="n">
+        <v>18012</v>
+      </c>
+      <c r="G31" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bq.gif</t>
         </is>
@@ -1291,7 +1481,13 @@
           <t>Brasilia</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="E32" t="n">
+        <v>8511965</v>
+      </c>
+      <c r="F32" t="n">
+        <v>209469333</v>
+      </c>
+      <c r="G32" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/br.gif</t>
         </is>
@@ -1318,7 +1514,13 @@
           <t>Nassau</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="E33" t="n">
+        <v>13940</v>
+      </c>
+      <c r="F33" t="n">
+        <v>385640</v>
+      </c>
+      <c r="G33" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bs.gif</t>
         </is>
@@ -1345,7 +1547,13 @@
           <t>Thimphu</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E34" t="n">
+        <v>47000</v>
+      </c>
+      <c r="F34" t="n">
+        <v>754394</v>
+      </c>
+      <c r="G34" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bt.gif</t>
         </is>
@@ -1372,7 +1580,13 @@
           <t>Ilha Bouvet</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="E35" t="n">
+        <v>49</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bv.gif</t>
         </is>
@@ -1399,7 +1613,13 @@
           <t>Gaborone</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="E36" t="n">
+        <v>600370</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2254126</v>
+      </c>
+      <c r="G36" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bw.gif</t>
         </is>
@@ -1426,7 +1646,13 @@
           <t>Minsk</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="E37" t="n">
+        <v>207600</v>
+      </c>
+      <c r="F37" t="n">
+        <v>9485386</v>
+      </c>
+      <c r="G37" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/by.gif</t>
         </is>
@@ -1453,7 +1679,13 @@
           <t>Belmopan</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="E38" t="n">
+        <v>22966</v>
+      </c>
+      <c r="F38" t="n">
+        <v>383071</v>
+      </c>
+      <c r="G38" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/bz.gif</t>
         </is>
@@ -1480,7 +1712,13 @@
           <t>Ottawa</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="E39" t="n">
+        <v>9984670</v>
+      </c>
+      <c r="F39" t="n">
+        <v>37058856</v>
+      </c>
+      <c r="G39" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ca.gif</t>
         </is>
@@ -1507,7 +1745,13 @@
           <t>West Island</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E40" t="n">
+        <v>14</v>
+      </c>
+      <c r="F40" t="n">
+        <v>628</v>
+      </c>
+      <c r="G40" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cc.gif</t>
         </is>
@@ -1534,7 +1778,13 @@
           <t>Kinshasa</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="E41" t="n">
+        <v>2345410</v>
+      </c>
+      <c r="F41" t="n">
+        <v>84068091</v>
+      </c>
+      <c r="G41" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cd.gif</t>
         </is>
@@ -1561,7 +1811,13 @@
           <t>Bangui</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="E42" t="n">
+        <v>622984</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4666377</v>
+      </c>
+      <c r="G42" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cf.gif</t>
         </is>
@@ -1588,7 +1844,13 @@
           <t>Brazzaville</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="E43" t="n">
+        <v>342000</v>
+      </c>
+      <c r="F43" t="n">
+        <v>5244363</v>
+      </c>
+      <c r="G43" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cg.gif</t>
         </is>
@@ -1615,7 +1877,13 @@
           <t>Bern</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="E44" t="n">
+        <v>41290</v>
+      </c>
+      <c r="F44" t="n">
+        <v>8516543</v>
+      </c>
+      <c r="G44" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ch.gif</t>
         </is>
@@ -1642,7 +1910,13 @@
           <t>Yamoussoukro</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="E45" t="n">
+        <v>322460</v>
+      </c>
+      <c r="F45" t="n">
+        <v>25069229</v>
+      </c>
+      <c r="G45" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ci.gif</t>
         </is>
@@ -1669,7 +1943,13 @@
           <t>Avarua</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="E46" t="n">
+        <v>240</v>
+      </c>
+      <c r="F46" t="n">
+        <v>21388</v>
+      </c>
+      <c r="G46" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ck.gif</t>
         </is>
@@ -1696,7 +1976,13 @@
           <t>Santiago</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E47" t="n">
+        <v>756950</v>
+      </c>
+      <c r="F47" t="n">
+        <v>18729160</v>
+      </c>
+      <c r="G47" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cl.gif</t>
         </is>
@@ -1723,7 +2009,13 @@
           <t>Yaounde</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="E48" t="n">
+        <v>475440</v>
+      </c>
+      <c r="F48" t="n">
+        <v>25216237</v>
+      </c>
+      <c r="G48" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cm.gif</t>
         </is>
@@ -1750,7 +2042,13 @@
           <t>Beijing</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="E49" t="n">
+        <v>9596960</v>
+      </c>
+      <c r="F49" t="n">
+        <v>1411778724</v>
+      </c>
+      <c r="G49" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cn.gif</t>
         </is>
@@ -1777,7 +2075,13 @@
           <t>Bogota</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="E50" t="n">
+        <v>1138910</v>
+      </c>
+      <c r="F50" t="n">
+        <v>49648685</v>
+      </c>
+      <c r="G50" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/co.gif</t>
         </is>
@@ -1804,7 +2108,13 @@
           <t>San Jose</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E51" t="n">
+        <v>51100</v>
+      </c>
+      <c r="F51" t="n">
+        <v>4999441</v>
+      </c>
+      <c r="G51" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cr.gif</t>
         </is>
@@ -1831,7 +2141,13 @@
           <t>Havana</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="E52" t="n">
+        <v>110860</v>
+      </c>
+      <c r="F52" t="n">
+        <v>11338138</v>
+      </c>
+      <c r="G52" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cu.gif</t>
         </is>
@@ -1858,7 +2174,13 @@
           <t>Praia</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="E53" t="n">
+        <v>4033</v>
+      </c>
+      <c r="F53" t="n">
+        <v>543767</v>
+      </c>
+      <c r="G53" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cv.gif</t>
         </is>
@@ -1885,7 +2207,13 @@
           <t>Willemstad</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="E54" t="n">
+        <v>444</v>
+      </c>
+      <c r="F54" t="n">
+        <v>159849</v>
+      </c>
+      <c r="G54" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cw.gif</t>
         </is>
@@ -1912,7 +2240,13 @@
           <t>Flying Fish Cove</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="E55" t="n">
+        <v>135</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G55" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cx.gif</t>
         </is>
@@ -1939,7 +2273,13 @@
           <t>Nicosia</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="E56" t="n">
+        <v>9250</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1189265</v>
+      </c>
+      <c r="G56" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cy.gif</t>
         </is>
@@ -1966,7 +2306,13 @@
           <t>Prague</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="E57" t="n">
+        <v>78866</v>
+      </c>
+      <c r="F57" t="n">
+        <v>10625695</v>
+      </c>
+      <c r="G57" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/cz.gif</t>
         </is>
@@ -1993,7 +2339,13 @@
           <t>Berlin</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="E58" t="n">
+        <v>357021</v>
+      </c>
+      <c r="F58" t="n">
+        <v>82927922</v>
+      </c>
+      <c r="G58" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/de.gif</t>
         </is>
@@ -2020,7 +2372,13 @@
           <t>Djibouti</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
+      <c r="E59" t="n">
+        <v>23000</v>
+      </c>
+      <c r="F59" t="n">
+        <v>958920</v>
+      </c>
+      <c r="G59" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/dj.gif</t>
         </is>
@@ -2047,7 +2405,13 @@
           <t>Copenhagen</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
+      <c r="E60" t="n">
+        <v>43094</v>
+      </c>
+      <c r="F60" t="n">
+        <v>5797446</v>
+      </c>
+      <c r="G60" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/dk.gif</t>
         </is>
@@ -2074,7 +2438,13 @@
           <t>Roseau</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
+      <c r="E61" t="n">
+        <v>754</v>
+      </c>
+      <c r="F61" t="n">
+        <v>71625</v>
+      </c>
+      <c r="G61" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/dm.gif</t>
         </is>
@@ -2101,7 +2471,13 @@
           <t>Santo Domingo</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
+      <c r="E62" t="n">
+        <v>48730</v>
+      </c>
+      <c r="F62" t="n">
+        <v>10627165</v>
+      </c>
+      <c r="G62" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/do.gif</t>
         </is>
@@ -2128,7 +2504,13 @@
           <t>Algiers</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="E63" t="n">
+        <v>2381740</v>
+      </c>
+      <c r="F63" t="n">
+        <v>42228429</v>
+      </c>
+      <c r="G63" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/dz.gif</t>
         </is>
@@ -2155,7 +2537,13 @@
           <t>Quito</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
+      <c r="E64" t="n">
+        <v>283560</v>
+      </c>
+      <c r="F64" t="n">
+        <v>17084357</v>
+      </c>
+      <c r="G64" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ec.gif</t>
         </is>
@@ -2182,7 +2570,13 @@
           <t>Tallinn</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
+      <c r="E65" t="n">
+        <v>45226</v>
+      </c>
+      <c r="F65" t="n">
+        <v>1320884</v>
+      </c>
+      <c r="G65" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ee.gif</t>
         </is>
@@ -2209,7 +2603,13 @@
           <t>Cairo</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
+      <c r="E66" t="n">
+        <v>1001450</v>
+      </c>
+      <c r="F66" t="n">
+        <v>98423595</v>
+      </c>
+      <c r="G66" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/eg.gif</t>
         </is>
@@ -2236,7 +2636,13 @@
           <t>El-Aaiun</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
+      <c r="E67" t="n">
+        <v>266000</v>
+      </c>
+      <c r="F67" t="n">
+        <v>273008</v>
+      </c>
+      <c r="G67" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/eh.gif</t>
         </is>
@@ -2263,7 +2669,13 @@
           <t>Asmara</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
+      <c r="E68" t="n">
+        <v>121320</v>
+      </c>
+      <c r="F68" t="n">
+        <v>6209262</v>
+      </c>
+      <c r="G68" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/er.gif</t>
         </is>
@@ -2290,7 +2702,13 @@
           <t>Madrid</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
+      <c r="E69" t="n">
+        <v>504782</v>
+      </c>
+      <c r="F69" t="n">
+        <v>46723749</v>
+      </c>
+      <c r="G69" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/es.gif</t>
         </is>
@@ -2317,7 +2735,13 @@
           <t>Addis Ababa</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
+      <c r="E70" t="n">
+        <v>1127127</v>
+      </c>
+      <c r="F70" t="n">
+        <v>109224559</v>
+      </c>
+      <c r="G70" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/et.gif</t>
         </is>
@@ -2344,7 +2768,13 @@
           <t>Helsinki</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
+      <c r="E71" t="n">
+        <v>337030</v>
+      </c>
+      <c r="F71" t="n">
+        <v>5518050</v>
+      </c>
+      <c r="G71" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/fi.gif</t>
         </is>
@@ -2371,7 +2801,13 @@
           <t>Suva</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
+      <c r="E72" t="n">
+        <v>18270</v>
+      </c>
+      <c r="F72" t="n">
+        <v>883483</v>
+      </c>
+      <c r="G72" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/fj.gif</t>
         </is>
@@ -2398,7 +2834,13 @@
           <t>Stanley</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="E73" t="n">
+        <v>12173</v>
+      </c>
+      <c r="F73" t="n">
+        <v>2638</v>
+      </c>
+      <c r="G73" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/fk.gif</t>
         </is>
@@ -2425,7 +2867,13 @@
           <t>Palikir</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
+      <c r="E74" t="n">
+        <v>702</v>
+      </c>
+      <c r="F74" t="n">
+        <v>112640</v>
+      </c>
+      <c r="G74" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/fm.gif</t>
         </is>
@@ -2452,7 +2900,13 @@
           <t>Torshavn</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
+      <c r="E75" t="n">
+        <v>1399</v>
+      </c>
+      <c r="F75" t="n">
+        <v>48497</v>
+      </c>
+      <c r="G75" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/fo.gif</t>
         </is>
@@ -2479,7 +2933,13 @@
           <t>Paris</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
+      <c r="E76" t="n">
+        <v>547030</v>
+      </c>
+      <c r="F76" t="n">
+        <v>66987244</v>
+      </c>
+      <c r="G76" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/fr.gif</t>
         </is>
@@ -2506,7 +2966,13 @@
           <t>Libreville</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr">
+      <c r="E77" t="n">
+        <v>267667</v>
+      </c>
+      <c r="F77" t="n">
+        <v>2119275</v>
+      </c>
+      <c r="G77" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ga.gif</t>
         </is>
@@ -2533,7 +2999,13 @@
           <t>London</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr">
+      <c r="E78" t="n">
+        <v>244820</v>
+      </c>
+      <c r="F78" t="n">
+        <v>66488991</v>
+      </c>
+      <c r="G78" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gb.gif</t>
         </is>
@@ -2560,7 +3032,13 @@
           <t>St. George's</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
+      <c r="E79" t="n">
+        <v>344</v>
+      </c>
+      <c r="F79" t="n">
+        <v>111454</v>
+      </c>
+      <c r="G79" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gd.gif</t>
         </is>
@@ -2587,7 +3065,13 @@
           <t>Tbilisi</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr">
+      <c r="E80" t="n">
+        <v>69700</v>
+      </c>
+      <c r="F80" t="n">
+        <v>3731000</v>
+      </c>
+      <c r="G80" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ge.gif</t>
         </is>
@@ -2614,7 +3098,13 @@
           <t>Cayenne</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr">
+      <c r="E81" t="n">
+        <v>91000</v>
+      </c>
+      <c r="F81" t="n">
+        <v>195506</v>
+      </c>
+      <c r="G81" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gf.gif</t>
         </is>
@@ -2641,7 +3131,13 @@
           <t>St Peter Port</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr">
+      <c r="E82" t="n">
+        <v>78</v>
+      </c>
+      <c r="F82" t="n">
+        <v>65228</v>
+      </c>
+      <c r="G82" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gg.gif</t>
         </is>
@@ -2668,7 +3164,13 @@
           <t>Accra</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr">
+      <c r="E83" t="n">
+        <v>239460</v>
+      </c>
+      <c r="F83" t="n">
+        <v>29767108</v>
+      </c>
+      <c r="G83" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gh.gif</t>
         </is>
@@ -2695,7 +3197,13 @@
           <t>Gibraltar</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr">
+      <c r="E84" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="F84" t="n">
+        <v>33718</v>
+      </c>
+      <c r="G84" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gi.gif</t>
         </is>
@@ -2722,7 +3230,13 @@
           <t>Nuuk</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr">
+      <c r="E85" t="n">
+        <v>2166086</v>
+      </c>
+      <c r="F85" t="n">
+        <v>56025</v>
+      </c>
+      <c r="G85" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gl.gif</t>
         </is>
@@ -2749,7 +3263,13 @@
           <t>Banjul</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr">
+      <c r="E86" t="n">
+        <v>11300</v>
+      </c>
+      <c r="F86" t="n">
+        <v>2280102</v>
+      </c>
+      <c r="G86" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gm.gif</t>
         </is>
@@ -2776,7 +3296,13 @@
           <t>Conakry</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr">
+      <c r="E87" t="n">
+        <v>245857</v>
+      </c>
+      <c r="F87" t="n">
+        <v>12414318</v>
+      </c>
+      <c r="G87" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gn.gif</t>
         </is>
@@ -2803,7 +3329,13 @@
           <t>Basse-Terre</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr">
+      <c r="E88" t="n">
+        <v>1780</v>
+      </c>
+      <c r="F88" t="n">
+        <v>443000</v>
+      </c>
+      <c r="G88" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gp.gif</t>
         </is>
@@ -2830,7 +3362,13 @@
           <t>Malabo</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr">
+      <c r="E89" t="n">
+        <v>28051</v>
+      </c>
+      <c r="F89" t="n">
+        <v>1308974</v>
+      </c>
+      <c r="G89" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gq.gif</t>
         </is>
@@ -2857,7 +3395,13 @@
           <t>Athens</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr">
+      <c r="E90" t="n">
+        <v>131940</v>
+      </c>
+      <c r="F90" t="n">
+        <v>10727668</v>
+      </c>
+      <c r="G90" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gr.gif</t>
         </is>
@@ -2884,7 +3428,13 @@
           <t>Grytviken</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr">
+      <c r="E91" t="n">
+        <v>3903</v>
+      </c>
+      <c r="F91" t="n">
+        <v>30</v>
+      </c>
+      <c r="G91" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gs.gif</t>
         </is>
@@ -2911,7 +3461,13 @@
           <t>Guatemala City</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr">
+      <c r="E92" t="n">
+        <v>108890</v>
+      </c>
+      <c r="F92" t="n">
+        <v>17247807</v>
+      </c>
+      <c r="G92" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gt.gif</t>
         </is>
@@ -2938,7 +3494,13 @@
           <t>Hagatna</t>
         </is>
       </c>
-      <c r="E93" t="inlineStr">
+      <c r="E93" t="n">
+        <v>549</v>
+      </c>
+      <c r="F93" t="n">
+        <v>165768</v>
+      </c>
+      <c r="G93" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gu.gif</t>
         </is>
@@ -2965,7 +3527,13 @@
           <t>Bissau</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr">
+      <c r="E94" t="n">
+        <v>36120</v>
+      </c>
+      <c r="F94" t="n">
+        <v>1874309</v>
+      </c>
+      <c r="G94" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gw.gif</t>
         </is>
@@ -2992,7 +3560,13 @@
           <t>Georgetown</t>
         </is>
       </c>
-      <c r="E95" t="inlineStr">
+      <c r="E95" t="n">
+        <v>214970</v>
+      </c>
+      <c r="F95" t="n">
+        <v>779004</v>
+      </c>
+      <c r="G95" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/gy.gif</t>
         </is>
@@ -3019,7 +3593,13 @@
           <t>Hong Kong</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr">
+      <c r="E96" t="n">
+        <v>1092</v>
+      </c>
+      <c r="F96" t="n">
+        <v>7491609</v>
+      </c>
+      <c r="G96" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/hk.gif</t>
         </is>
@@ -3046,7 +3626,13 @@
           <t>Ilhas Heard e McDonald</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr">
+      <c r="E97" t="n">
+        <v>412</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0</v>
+      </c>
+      <c r="G97" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/hm.gif</t>
         </is>
@@ -3073,7 +3659,13 @@
           <t>Tegucigalpa</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr">
+      <c r="E98" t="n">
+        <v>112090</v>
+      </c>
+      <c r="F98" t="n">
+        <v>9587522</v>
+      </c>
+      <c r="G98" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/hn.gif</t>
         </is>
@@ -3100,7 +3692,13 @@
           <t>Zagreb</t>
         </is>
       </c>
-      <c r="E99" t="inlineStr">
+      <c r="E99" t="n">
+        <v>56542</v>
+      </c>
+      <c r="F99" t="n">
+        <v>3871833</v>
+      </c>
+      <c r="G99" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/hr.gif</t>
         </is>
@@ -3127,7 +3725,13 @@
           <t>Port-au-Prince</t>
         </is>
       </c>
-      <c r="E100" t="inlineStr">
+      <c r="E100" t="n">
+        <v>27750</v>
+      </c>
+      <c r="F100" t="n">
+        <v>11123176</v>
+      </c>
+      <c r="G100" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ht.gif</t>
         </is>
@@ -3154,7 +3758,13 @@
           <t>Budapest</t>
         </is>
       </c>
-      <c r="E101" t="inlineStr">
+      <c r="E101" t="n">
+        <v>93030</v>
+      </c>
+      <c r="F101" t="n">
+        <v>9768785</v>
+      </c>
+      <c r="G101" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/hu.gif</t>
         </is>
@@ -3181,7 +3791,13 @@
           <t>Jakarta</t>
         </is>
       </c>
-      <c r="E102" t="inlineStr">
+      <c r="E102" t="n">
+        <v>1919440</v>
+      </c>
+      <c r="F102" t="n">
+        <v>267663435</v>
+      </c>
+      <c r="G102" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/id.gif</t>
         </is>
@@ -3208,7 +3824,13 @@
           <t>Dublin</t>
         </is>
       </c>
-      <c r="E103" t="inlineStr">
+      <c r="E103" t="n">
+        <v>70280</v>
+      </c>
+      <c r="F103" t="n">
+        <v>4853506</v>
+      </c>
+      <c r="G103" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ie.gif</t>
         </is>
@@ -3235,7 +3857,13 @@
           <t>Jerusalem</t>
         </is>
       </c>
-      <c r="E104" t="inlineStr">
+      <c r="E104" t="n">
+        <v>20770</v>
+      </c>
+      <c r="F104" t="n">
+        <v>8883800</v>
+      </c>
+      <c r="G104" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/il.gif</t>
         </is>
@@ -3262,7 +3890,13 @@
           <t>Douglas</t>
         </is>
       </c>
-      <c r="E105" t="inlineStr">
+      <c r="E105" t="n">
+        <v>572</v>
+      </c>
+      <c r="F105" t="n">
+        <v>84077</v>
+      </c>
+      <c r="G105" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/im.gif</t>
         </is>
@@ -3289,7 +3923,13 @@
           <t>New Delhi</t>
         </is>
       </c>
-      <c r="E106" t="inlineStr">
+      <c r="E106" t="n">
+        <v>3287590</v>
+      </c>
+      <c r="F106" t="n">
+        <v>1352617328</v>
+      </c>
+      <c r="G106" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/in.gif</t>
         </is>
@@ -3316,7 +3956,13 @@
           <t>Diego Garcia</t>
         </is>
       </c>
-      <c r="E107" t="inlineStr">
+      <c r="E107" t="n">
+        <v>60</v>
+      </c>
+      <c r="F107" t="n">
+        <v>4000</v>
+      </c>
+      <c r="G107" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/io.gif</t>
         </is>
@@ -3343,7 +3989,13 @@
           <t>Baghdad</t>
         </is>
       </c>
-      <c r="E108" t="inlineStr">
+      <c r="E108" t="n">
+        <v>437072</v>
+      </c>
+      <c r="F108" t="n">
+        <v>38433600</v>
+      </c>
+      <c r="G108" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/iq.gif</t>
         </is>
@@ -3370,7 +4022,13 @@
           <t>Tehran</t>
         </is>
       </c>
-      <c r="E109" t="inlineStr">
+      <c r="E109" t="n">
+        <v>1648000</v>
+      </c>
+      <c r="F109" t="n">
+        <v>81800269</v>
+      </c>
+      <c r="G109" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ir.gif</t>
         </is>
@@ -3397,7 +4055,13 @@
           <t>Reykjavik</t>
         </is>
       </c>
-      <c r="E110" t="inlineStr">
+      <c r="E110" t="n">
+        <v>103000</v>
+      </c>
+      <c r="F110" t="n">
+        <v>353574</v>
+      </c>
+      <c r="G110" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/is.gif</t>
         </is>
@@ -3424,7 +4088,13 @@
           <t>Rome</t>
         </is>
       </c>
-      <c r="E111" t="inlineStr">
+      <c r="E111" t="n">
+        <v>301230</v>
+      </c>
+      <c r="F111" t="n">
+        <v>60431283</v>
+      </c>
+      <c r="G111" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/it.gif</t>
         </is>
@@ -3451,7 +4121,13 @@
           <t>Saint Helier</t>
         </is>
       </c>
-      <c r="E112" t="inlineStr">
+      <c r="E112" t="n">
+        <v>116</v>
+      </c>
+      <c r="F112" t="n">
+        <v>90812</v>
+      </c>
+      <c r="G112" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/je.gif</t>
         </is>
@@ -3478,7 +4154,13 @@
           <t>Kingston</t>
         </is>
       </c>
-      <c r="E113" t="inlineStr">
+      <c r="E113" t="n">
+        <v>10991</v>
+      </c>
+      <c r="F113" t="n">
+        <v>2934855</v>
+      </c>
+      <c r="G113" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/jm.gif</t>
         </is>
@@ -3505,7 +4187,13 @@
           <t>Amman</t>
         </is>
       </c>
-      <c r="E114" t="inlineStr">
+      <c r="E114" t="n">
+        <v>92300</v>
+      </c>
+      <c r="F114" t="n">
+        <v>9956011</v>
+      </c>
+      <c r="G114" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/jo.gif</t>
         </is>
@@ -3532,7 +4220,13 @@
           <t>Tokyo</t>
         </is>
       </c>
-      <c r="E115" t="inlineStr">
+      <c r="E115" t="n">
+        <v>377835</v>
+      </c>
+      <c r="F115" t="n">
+        <v>126529100</v>
+      </c>
+      <c r="G115" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/jp.gif</t>
         </is>
@@ -3559,7 +4253,13 @@
           <t>Nairobi</t>
         </is>
       </c>
-      <c r="E116" t="inlineStr">
+      <c r="E116" t="n">
+        <v>582650</v>
+      </c>
+      <c r="F116" t="n">
+        <v>51393010</v>
+      </c>
+      <c r="G116" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ke.gif</t>
         </is>
@@ -3586,7 +4286,13 @@
           <t>Bishkek</t>
         </is>
       </c>
-      <c r="E117" t="inlineStr">
+      <c r="E117" t="n">
+        <v>198500</v>
+      </c>
+      <c r="F117" t="n">
+        <v>6315800</v>
+      </c>
+      <c r="G117" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/kg.gif</t>
         </is>
@@ -3613,7 +4319,13 @@
           <t>Phnom Penh</t>
         </is>
       </c>
-      <c r="E118" t="inlineStr">
+      <c r="E118" t="n">
+        <v>181040</v>
+      </c>
+      <c r="F118" t="n">
+        <v>16249798</v>
+      </c>
+      <c r="G118" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/kh.gif</t>
         </is>
@@ -3640,7 +4352,13 @@
           <t>Tarawa</t>
         </is>
       </c>
-      <c r="E119" t="inlineStr">
+      <c r="E119" t="n">
+        <v>811</v>
+      </c>
+      <c r="F119" t="n">
+        <v>115847</v>
+      </c>
+      <c r="G119" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ki.gif</t>
         </is>
@@ -3667,7 +4385,13 @@
           <t>Moroni</t>
         </is>
       </c>
-      <c r="E120" t="inlineStr">
+      <c r="E120" t="n">
+        <v>2170</v>
+      </c>
+      <c r="F120" t="n">
+        <v>832322</v>
+      </c>
+      <c r="G120" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/km.gif</t>
         </is>
@@ -3694,7 +4418,13 @@
           <t>Basseterre</t>
         </is>
       </c>
-      <c r="E121" t="inlineStr">
+      <c r="E121" t="n">
+        <v>261</v>
+      </c>
+      <c r="F121" t="n">
+        <v>52441</v>
+      </c>
+      <c r="G121" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/kn.gif</t>
         </is>
@@ -3721,7 +4451,13 @@
           <t>Pyongyang</t>
         </is>
       </c>
-      <c r="E122" t="inlineStr">
+      <c r="E122" t="n">
+        <v>120540</v>
+      </c>
+      <c r="F122" t="n">
+        <v>25549819</v>
+      </c>
+      <c r="G122" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/kp.gif</t>
         </is>
@@ -3748,7 +4484,13 @@
           <t>Seoul</t>
         </is>
       </c>
-      <c r="E123" t="inlineStr">
+      <c r="E123" t="n">
+        <v>98480</v>
+      </c>
+      <c r="F123" t="n">
+        <v>51635256</v>
+      </c>
+      <c r="G123" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/kr.gif</t>
         </is>
@@ -3775,7 +4517,13 @@
           <t>Kuwait City</t>
         </is>
       </c>
-      <c r="E124" t="inlineStr">
+      <c r="E124" t="n">
+        <v>17820</v>
+      </c>
+      <c r="F124" t="n">
+        <v>4137309</v>
+      </c>
+      <c r="G124" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/kw.gif</t>
         </is>
@@ -3802,7 +4550,13 @@
           <t>George Town</t>
         </is>
       </c>
-      <c r="E125" t="inlineStr">
+      <c r="E125" t="n">
+        <v>262</v>
+      </c>
+      <c r="F125" t="n">
+        <v>64174</v>
+      </c>
+      <c r="G125" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ky.gif</t>
         </is>
@@ -3829,7 +4583,13 @@
           <t>Nur-Sultan</t>
         </is>
       </c>
-      <c r="E126" t="inlineStr">
+      <c r="E126" t="n">
+        <v>2717300</v>
+      </c>
+      <c r="F126" t="n">
+        <v>18276499</v>
+      </c>
+      <c r="G126" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/kz.gif</t>
         </is>
@@ -3856,7 +4616,13 @@
           <t>Vientiane</t>
         </is>
       </c>
-      <c r="E127" t="inlineStr">
+      <c r="E127" t="n">
+        <v>236800</v>
+      </c>
+      <c r="F127" t="n">
+        <v>7061507</v>
+      </c>
+      <c r="G127" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/la.gif</t>
         </is>
@@ -3883,7 +4649,13 @@
           <t>Beirut</t>
         </is>
       </c>
-      <c r="E128" t="inlineStr">
+      <c r="E128" t="n">
+        <v>10400</v>
+      </c>
+      <c r="F128" t="n">
+        <v>6848925</v>
+      </c>
+      <c r="G128" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/lb.gif</t>
         </is>
@@ -3910,7 +4682,13 @@
           <t>Castries</t>
         </is>
       </c>
-      <c r="E129" t="inlineStr">
+      <c r="E129" t="n">
+        <v>616</v>
+      </c>
+      <c r="F129" t="n">
+        <v>181889</v>
+      </c>
+      <c r="G129" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/lc.gif</t>
         </is>
@@ -3937,7 +4715,13 @@
           <t>Vaduz</t>
         </is>
       </c>
-      <c r="E130" t="inlineStr">
+      <c r="E130" t="n">
+        <v>160</v>
+      </c>
+      <c r="F130" t="n">
+        <v>37910</v>
+      </c>
+      <c r="G130" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/li.gif</t>
         </is>
@@ -3964,7 +4748,13 @@
           <t>Colombo</t>
         </is>
       </c>
-      <c r="E131" t="inlineStr">
+      <c r="E131" t="n">
+        <v>65610</v>
+      </c>
+      <c r="F131" t="n">
+        <v>21670000</v>
+      </c>
+      <c r="G131" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/lk.gif</t>
         </is>
@@ -3991,7 +4781,13 @@
           <t>Monrovia</t>
         </is>
       </c>
-      <c r="E132" t="inlineStr">
+      <c r="E132" t="n">
+        <v>111370</v>
+      </c>
+      <c r="F132" t="n">
+        <v>4818977</v>
+      </c>
+      <c r="G132" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/lr.gif</t>
         </is>
@@ -4018,7 +4814,13 @@
           <t>Maseru</t>
         </is>
       </c>
-      <c r="E133" t="inlineStr">
+      <c r="E133" t="n">
+        <v>30355</v>
+      </c>
+      <c r="F133" t="n">
+        <v>2108132</v>
+      </c>
+      <c r="G133" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ls.gif</t>
         </is>
@@ -4045,7 +4847,13 @@
           <t>Vilnius</t>
         </is>
       </c>
-      <c r="E134" t="inlineStr">
+      <c r="E134" t="n">
+        <v>65200</v>
+      </c>
+      <c r="F134" t="n">
+        <v>2789533</v>
+      </c>
+      <c r="G134" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/lt.gif</t>
         </is>
@@ -4072,7 +4880,13 @@
           <t>Luxembourg</t>
         </is>
       </c>
-      <c r="E135" t="inlineStr">
+      <c r="E135" t="n">
+        <v>2586</v>
+      </c>
+      <c r="F135" t="n">
+        <v>607728</v>
+      </c>
+      <c r="G135" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/lu.gif</t>
         </is>
@@ -4099,7 +4913,13 @@
           <t>Riga</t>
         </is>
       </c>
-      <c r="E136" t="inlineStr">
+      <c r="E136" t="n">
+        <v>64589</v>
+      </c>
+      <c r="F136" t="n">
+        <v>1926542</v>
+      </c>
+      <c r="G136" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/lv.gif</t>
         </is>
@@ -4126,7 +4946,13 @@
           <t>Tripoli</t>
         </is>
       </c>
-      <c r="E137" t="inlineStr">
+      <c r="E137" t="n">
+        <v>1759540</v>
+      </c>
+      <c r="F137" t="n">
+        <v>6678567</v>
+      </c>
+      <c r="G137" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ly.gif</t>
         </is>
@@ -4153,7 +4979,13 @@
           <t>Rabat</t>
         </is>
       </c>
-      <c r="E138" t="inlineStr">
+      <c r="E138" t="n">
+        <v>446550</v>
+      </c>
+      <c r="F138" t="n">
+        <v>36029138</v>
+      </c>
+      <c r="G138" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ma.gif</t>
         </is>
@@ -4180,7 +5012,13 @@
           <t>Monaco</t>
         </is>
       </c>
-      <c r="E139" t="inlineStr">
+      <c r="E139" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="F139" t="n">
+        <v>38682</v>
+      </c>
+      <c r="G139" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mc.gif</t>
         </is>
@@ -4207,7 +5045,13 @@
           <t>Chisinau</t>
         </is>
       </c>
-      <c r="E140" t="inlineStr">
+      <c r="E140" t="n">
+        <v>33843</v>
+      </c>
+      <c r="F140" t="n">
+        <v>3545883</v>
+      </c>
+      <c r="G140" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/md.gif</t>
         </is>
@@ -4234,7 +5078,13 @@
           <t>Podgorica</t>
         </is>
       </c>
-      <c r="E141" t="inlineStr">
+      <c r="E141" t="n">
+        <v>14026</v>
+      </c>
+      <c r="F141" t="n">
+        <v>622345</v>
+      </c>
+      <c r="G141" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/me.gif</t>
         </is>
@@ -4261,7 +5111,13 @@
           <t>Marigot</t>
         </is>
       </c>
-      <c r="E142" t="inlineStr">
+      <c r="E142" t="n">
+        <v>53</v>
+      </c>
+      <c r="F142" t="n">
+        <v>37264</v>
+      </c>
+      <c r="G142" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mf.gif</t>
         </is>
@@ -4288,7 +5144,13 @@
           <t>Antananarivo</t>
         </is>
       </c>
-      <c r="E143" t="inlineStr">
+      <c r="E143" t="n">
+        <v>587040</v>
+      </c>
+      <c r="F143" t="n">
+        <v>26262368</v>
+      </c>
+      <c r="G143" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mg.gif</t>
         </is>
@@ -4315,7 +5177,13 @@
           <t>Majuro</t>
         </is>
       </c>
-      <c r="E144" t="inlineStr">
+      <c r="E144" t="n">
+        <v>181.3</v>
+      </c>
+      <c r="F144" t="n">
+        <v>58413</v>
+      </c>
+      <c r="G144" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mh.gif</t>
         </is>
@@ -4342,7 +5210,13 @@
           <t>Skopje</t>
         </is>
       </c>
-      <c r="E145" t="inlineStr">
+      <c r="E145" t="n">
+        <v>25333</v>
+      </c>
+      <c r="F145" t="n">
+        <v>2082958</v>
+      </c>
+      <c r="G145" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mk.gif</t>
         </is>
@@ -4369,7 +5243,13 @@
           <t>Bamako</t>
         </is>
       </c>
-      <c r="E146" t="inlineStr">
+      <c r="E146" t="n">
+        <v>1240000</v>
+      </c>
+      <c r="F146" t="n">
+        <v>19077690</v>
+      </c>
+      <c r="G146" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ml.gif</t>
         </is>
@@ -4396,7 +5276,13 @@
           <t>Nay Pyi Taw</t>
         </is>
       </c>
-      <c r="E147" t="inlineStr">
+      <c r="E147" t="n">
+        <v>678500</v>
+      </c>
+      <c r="F147" t="n">
+        <v>53708395</v>
+      </c>
+      <c r="G147" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mm.gif</t>
         </is>
@@ -4423,7 +5309,13 @@
           <t>Ulaanbaatar</t>
         </is>
       </c>
-      <c r="E148" t="inlineStr">
+      <c r="E148" t="n">
+        <v>1565000</v>
+      </c>
+      <c r="F148" t="n">
+        <v>3170208</v>
+      </c>
+      <c r="G148" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mn.gif</t>
         </is>
@@ -4450,7 +5342,13 @@
           <t>Macao</t>
         </is>
       </c>
-      <c r="E149" t="inlineStr">
+      <c r="E149" t="n">
+        <v>254</v>
+      </c>
+      <c r="F149" t="n">
+        <v>631636</v>
+      </c>
+      <c r="G149" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mo.gif</t>
         </is>
@@ -4477,7 +5375,13 @@
           <t>Saipan</t>
         </is>
       </c>
-      <c r="E150" t="inlineStr">
+      <c r="E150" t="n">
+        <v>477</v>
+      </c>
+      <c r="F150" t="n">
+        <v>56882</v>
+      </c>
+      <c r="G150" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mp.gif</t>
         </is>
@@ -4504,7 +5408,13 @@
           <t>Fort-de-France</t>
         </is>
       </c>
-      <c r="E151" t="inlineStr">
+      <c r="E151" t="n">
+        <v>1100</v>
+      </c>
+      <c r="F151" t="n">
+        <v>432900</v>
+      </c>
+      <c r="G151" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mq.gif</t>
         </is>
@@ -4531,7 +5441,13 @@
           <t>Nouakchott</t>
         </is>
       </c>
-      <c r="E152" t="inlineStr">
+      <c r="E152" t="n">
+        <v>1030700</v>
+      </c>
+      <c r="F152" t="n">
+        <v>4403319</v>
+      </c>
+      <c r="G152" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mr.gif</t>
         </is>
@@ -4558,7 +5474,13 @@
           <t>Plymouth</t>
         </is>
       </c>
-      <c r="E153" t="inlineStr">
+      <c r="E153" t="n">
+        <v>102</v>
+      </c>
+      <c r="F153" t="n">
+        <v>9341</v>
+      </c>
+      <c r="G153" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ms.gif</t>
         </is>
@@ -4585,7 +5507,13 @@
           <t>Valletta</t>
         </is>
       </c>
-      <c r="E154" t="inlineStr">
+      <c r="E154" t="n">
+        <v>316</v>
+      </c>
+      <c r="F154" t="n">
+        <v>483530</v>
+      </c>
+      <c r="G154" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mt.gif</t>
         </is>
@@ -4612,7 +5540,13 @@
           <t>Port Louis</t>
         </is>
       </c>
-      <c r="E155" t="inlineStr">
+      <c r="E155" t="n">
+        <v>2040</v>
+      </c>
+      <c r="F155" t="n">
+        <v>1265303</v>
+      </c>
+      <c r="G155" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mu.gif</t>
         </is>
@@ -4639,7 +5573,13 @@
           <t>Male</t>
         </is>
       </c>
-      <c r="E156" t="inlineStr">
+      <c r="E156" t="n">
+        <v>300</v>
+      </c>
+      <c r="F156" t="n">
+        <v>515696</v>
+      </c>
+      <c r="G156" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mv.gif</t>
         </is>
@@ -4666,7 +5606,13 @@
           <t>Lilongwe</t>
         </is>
       </c>
-      <c r="E157" t="inlineStr">
+      <c r="E157" t="n">
+        <v>118480</v>
+      </c>
+      <c r="F157" t="n">
+        <v>17563749</v>
+      </c>
+      <c r="G157" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mw.gif</t>
         </is>
@@ -4693,7 +5639,13 @@
           <t>Mexico City</t>
         </is>
       </c>
-      <c r="E158" t="inlineStr">
+      <c r="E158" t="n">
+        <v>1972550</v>
+      </c>
+      <c r="F158" t="n">
+        <v>126190788</v>
+      </c>
+      <c r="G158" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mx.gif</t>
         </is>
@@ -4720,7 +5672,13 @@
           <t>Kuala Lumpur</t>
         </is>
       </c>
-      <c r="E159" t="inlineStr">
+      <c r="E159" t="n">
+        <v>329750</v>
+      </c>
+      <c r="F159" t="n">
+        <v>31528585</v>
+      </c>
+      <c r="G159" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/my.gif</t>
         </is>
@@ -4747,7 +5705,13 @@
           <t>Maputo</t>
         </is>
       </c>
-      <c r="E160" t="inlineStr">
+      <c r="E160" t="n">
+        <v>801590</v>
+      </c>
+      <c r="F160" t="n">
+        <v>29495962</v>
+      </c>
+      <c r="G160" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/mz.gif</t>
         </is>
@@ -4774,7 +5738,13 @@
           <t>Windhoek</t>
         </is>
       </c>
-      <c r="E161" t="inlineStr">
+      <c r="E161" t="n">
+        <v>825418</v>
+      </c>
+      <c r="F161" t="n">
+        <v>2448255</v>
+      </c>
+      <c r="G161" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/na.gif</t>
         </is>
@@ -4801,7 +5771,13 @@
           <t>Noumea</t>
         </is>
       </c>
-      <c r="E162" t="inlineStr">
+      <c r="E162" t="n">
+        <v>19060</v>
+      </c>
+      <c r="F162" t="n">
+        <v>284060</v>
+      </c>
+      <c r="G162" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/nc.gif</t>
         </is>
@@ -4828,7 +5804,13 @@
           <t>Niamey</t>
         </is>
       </c>
-      <c r="E163" t="inlineStr">
+      <c r="E163" t="n">
+        <v>1267000</v>
+      </c>
+      <c r="F163" t="n">
+        <v>22442948</v>
+      </c>
+      <c r="G163" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ne.gif</t>
         </is>
@@ -4855,7 +5837,13 @@
           <t>Kingston</t>
         </is>
       </c>
-      <c r="E164" t="inlineStr">
+      <c r="E164" t="n">
+        <v>34.6</v>
+      </c>
+      <c r="F164" t="n">
+        <v>1828</v>
+      </c>
+      <c r="G164" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/nf.gif</t>
         </is>
@@ -4882,7 +5870,13 @@
           <t>Abuja</t>
         </is>
       </c>
-      <c r="E165" t="inlineStr">
+      <c r="E165" t="n">
+        <v>923768</v>
+      </c>
+      <c r="F165" t="n">
+        <v>195874740</v>
+      </c>
+      <c r="G165" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ng.gif</t>
         </is>
@@ -4909,7 +5903,13 @@
           <t>Managua</t>
         </is>
       </c>
-      <c r="E166" t="inlineStr">
+      <c r="E166" t="n">
+        <v>129494</v>
+      </c>
+      <c r="F166" t="n">
+        <v>6465513</v>
+      </c>
+      <c r="G166" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ni.gif</t>
         </is>
@@ -4936,7 +5936,13 @@
           <t>Amsterdam</t>
         </is>
       </c>
-      <c r="E167" t="inlineStr">
+      <c r="E167" t="n">
+        <v>41526</v>
+      </c>
+      <c r="F167" t="n">
+        <v>17231017</v>
+      </c>
+      <c r="G167" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/nl.gif</t>
         </is>
@@ -4963,7 +5969,13 @@
           <t>Oslo</t>
         </is>
       </c>
-      <c r="E168" t="inlineStr">
+      <c r="E168" t="n">
+        <v>324220</v>
+      </c>
+      <c r="F168" t="n">
+        <v>5314336</v>
+      </c>
+      <c r="G168" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/no.gif</t>
         </is>
@@ -4990,7 +6002,13 @@
           <t>Kathmandu</t>
         </is>
       </c>
-      <c r="E169" t="inlineStr">
+      <c r="E169" t="n">
+        <v>140800</v>
+      </c>
+      <c r="F169" t="n">
+        <v>28087871</v>
+      </c>
+      <c r="G169" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/np.gif</t>
         </is>
@@ -5017,7 +6035,13 @@
           <t>Yaren</t>
         </is>
       </c>
-      <c r="E170" t="inlineStr">
+      <c r="E170" t="n">
+        <v>21</v>
+      </c>
+      <c r="F170" t="n">
+        <v>12704</v>
+      </c>
+      <c r="G170" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/nr.gif</t>
         </is>
@@ -5044,7 +6068,13 @@
           <t>Alofi</t>
         </is>
       </c>
-      <c r="E171" t="inlineStr">
+      <c r="E171" t="n">
+        <v>260</v>
+      </c>
+      <c r="F171" t="n">
+        <v>2166</v>
+      </c>
+      <c r="G171" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/nu.gif</t>
         </is>
@@ -5071,7 +6101,13 @@
           <t>Wellington</t>
         </is>
       </c>
-      <c r="E172" t="inlineStr">
+      <c r="E172" t="n">
+        <v>268680</v>
+      </c>
+      <c r="F172" t="n">
+        <v>4885500</v>
+      </c>
+      <c r="G172" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/nz.gif</t>
         </is>
@@ -5098,7 +6134,13 @@
           <t>Muscat</t>
         </is>
       </c>
-      <c r="E173" t="inlineStr">
+      <c r="E173" t="n">
+        <v>212460</v>
+      </c>
+      <c r="F173" t="n">
+        <v>4829483</v>
+      </c>
+      <c r="G173" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/om.gif</t>
         </is>
@@ -5125,7 +6167,13 @@
           <t>Panama City</t>
         </is>
       </c>
-      <c r="E174" t="inlineStr">
+      <c r="E174" t="n">
+        <v>78200</v>
+      </c>
+      <c r="F174" t="n">
+        <v>4176873</v>
+      </c>
+      <c r="G174" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/pa.gif</t>
         </is>
@@ -5152,7 +6200,13 @@
           <t>Lima</t>
         </is>
       </c>
-      <c r="E175" t="inlineStr">
+      <c r="E175" t="n">
+        <v>1285220</v>
+      </c>
+      <c r="F175" t="n">
+        <v>31989256</v>
+      </c>
+      <c r="G175" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/pe.gif</t>
         </is>
@@ -5179,7 +6233,13 @@
           <t>Papeete</t>
         </is>
       </c>
-      <c r="E176" t="inlineStr">
+      <c r="E176" t="n">
+        <v>4167</v>
+      </c>
+      <c r="F176" t="n">
+        <v>277679</v>
+      </c>
+      <c r="G176" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/pf.gif</t>
         </is>
@@ -5206,7 +6266,13 @@
           <t>Port Moresby</t>
         </is>
       </c>
-      <c r="E177" t="inlineStr">
+      <c r="E177" t="n">
+        <v>462840</v>
+      </c>
+      <c r="F177" t="n">
+        <v>8606316</v>
+      </c>
+      <c r="G177" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/pg.gif</t>
         </is>
@@ -5233,7 +6299,13 @@
           <t>Manila</t>
         </is>
       </c>
-      <c r="E178" t="inlineStr">
+      <c r="E178" t="n">
+        <v>300000</v>
+      </c>
+      <c r="F178" t="n">
+        <v>106651922</v>
+      </c>
+      <c r="G178" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ph.gif</t>
         </is>
@@ -5260,7 +6332,13 @@
           <t>Islamabad</t>
         </is>
       </c>
-      <c r="E179" t="inlineStr">
+      <c r="E179" t="n">
+        <v>803940</v>
+      </c>
+      <c r="F179" t="n">
+        <v>212215030</v>
+      </c>
+      <c r="G179" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/pk.gif</t>
         </is>
@@ -5287,7 +6365,13 @@
           <t>Warsaw</t>
         </is>
       </c>
-      <c r="E180" t="inlineStr">
+      <c r="E180" t="n">
+        <v>312685</v>
+      </c>
+      <c r="F180" t="n">
+        <v>37978548</v>
+      </c>
+      <c r="G180" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/pl.gif</t>
         </is>
@@ -5314,7 +6398,13 @@
           <t>Saint-Pierre</t>
         </is>
       </c>
-      <c r="E181" t="inlineStr">
+      <c r="E181" t="n">
+        <v>242</v>
+      </c>
+      <c r="F181" t="n">
+        <v>7012</v>
+      </c>
+      <c r="G181" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/pm.gif</t>
         </is>
@@ -5341,7 +6431,13 @@
           <t>Adamstown</t>
         </is>
       </c>
-      <c r="E182" t="inlineStr">
+      <c r="E182" t="n">
+        <v>47</v>
+      </c>
+      <c r="F182" t="n">
+        <v>46</v>
+      </c>
+      <c r="G182" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/pn.gif</t>
         </is>
@@ -5368,7 +6464,13 @@
           <t>San Juan</t>
         </is>
       </c>
-      <c r="E183" t="inlineStr">
+      <c r="E183" t="n">
+        <v>9104</v>
+      </c>
+      <c r="F183" t="n">
+        <v>3195153</v>
+      </c>
+      <c r="G183" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/pr.gif</t>
         </is>
@@ -5395,7 +6497,13 @@
           <t>East Jerusalem</t>
         </is>
       </c>
-      <c r="E184" t="inlineStr">
+      <c r="E184" t="n">
+        <v>5970</v>
+      </c>
+      <c r="F184" t="n">
+        <v>4569087</v>
+      </c>
+      <c r="G184" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ps.gif</t>
         </is>
@@ -5422,7 +6530,13 @@
           <t>Lisbon</t>
         </is>
       </c>
-      <c r="E185" t="inlineStr">
+      <c r="E185" t="n">
+        <v>92391</v>
+      </c>
+      <c r="F185" t="n">
+        <v>10281762</v>
+      </c>
+      <c r="G185" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/pt.gif</t>
         </is>
@@ -5449,7 +6563,13 @@
           <t>Melekeok</t>
         </is>
       </c>
-      <c r="E186" t="inlineStr">
+      <c r="E186" t="n">
+        <v>458</v>
+      </c>
+      <c r="F186" t="n">
+        <v>17907</v>
+      </c>
+      <c r="G186" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/pw.gif</t>
         </is>
@@ -5476,7 +6596,13 @@
           <t>Asuncion</t>
         </is>
       </c>
-      <c r="E187" t="inlineStr">
+      <c r="E187" t="n">
+        <v>406750</v>
+      </c>
+      <c r="F187" t="n">
+        <v>6956071</v>
+      </c>
+      <c r="G187" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/py.gif</t>
         </is>
@@ -5503,7 +6629,13 @@
           <t>Doha</t>
         </is>
       </c>
-      <c r="E188" t="inlineStr">
+      <c r="E188" t="n">
+        <v>11437</v>
+      </c>
+      <c r="F188" t="n">
+        <v>2781677</v>
+      </c>
+      <c r="G188" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/qa.gif</t>
         </is>
@@ -5530,7 +6662,13 @@
           <t>Saint-Denis</t>
         </is>
       </c>
-      <c r="E189" t="inlineStr">
+      <c r="E189" t="n">
+        <v>2517</v>
+      </c>
+      <c r="F189" t="n">
+        <v>776948</v>
+      </c>
+      <c r="G189" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/re.gif</t>
         </is>
@@ -5557,7 +6695,13 @@
           <t>Bucharest</t>
         </is>
       </c>
-      <c r="E190" t="inlineStr">
+      <c r="E190" t="n">
+        <v>237500</v>
+      </c>
+      <c r="F190" t="n">
+        <v>19473936</v>
+      </c>
+      <c r="G190" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ro.gif</t>
         </is>
@@ -5584,7 +6728,13 @@
           <t>Belgrade</t>
         </is>
       </c>
-      <c r="E191" t="inlineStr">
+      <c r="E191" t="n">
+        <v>88361</v>
+      </c>
+      <c r="F191" t="n">
+        <v>6982084</v>
+      </c>
+      <c r="G191" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/rs.gif</t>
         </is>
@@ -5611,7 +6761,13 @@
           <t>Moscow</t>
         </is>
       </c>
-      <c r="E192" t="inlineStr">
+      <c r="E192" t="n">
+        <v>17100000</v>
+      </c>
+      <c r="F192" t="n">
+        <v>144478050</v>
+      </c>
+      <c r="G192" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ru.gif</t>
         </is>
@@ -5638,7 +6794,13 @@
           <t>Kigali</t>
         </is>
       </c>
-      <c r="E193" t="inlineStr">
+      <c r="E193" t="n">
+        <v>26338</v>
+      </c>
+      <c r="F193" t="n">
+        <v>12301939</v>
+      </c>
+      <c r="G193" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/rw.gif</t>
         </is>
@@ -5665,7 +6827,13 @@
           <t>Riyadh</t>
         </is>
       </c>
-      <c r="E194" t="inlineStr">
+      <c r="E194" t="n">
+        <v>1960582</v>
+      </c>
+      <c r="F194" t="n">
+        <v>33699947</v>
+      </c>
+      <c r="G194" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sa.gif</t>
         </is>
@@ -5692,7 +6860,13 @@
           <t>Honiara</t>
         </is>
       </c>
-      <c r="E195" t="inlineStr">
+      <c r="E195" t="n">
+        <v>28450</v>
+      </c>
+      <c r="F195" t="n">
+        <v>652858</v>
+      </c>
+      <c r="G195" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sb.gif</t>
         </is>
@@ -5719,7 +6893,13 @@
           <t>Victoria</t>
         </is>
       </c>
-      <c r="E196" t="inlineStr">
+      <c r="E196" t="n">
+        <v>455</v>
+      </c>
+      <c r="F196" t="n">
+        <v>96762</v>
+      </c>
+      <c r="G196" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sc.gif</t>
         </is>
@@ -5746,7 +6926,13 @@
           <t>Khartoum</t>
         </is>
       </c>
-      <c r="E197" t="inlineStr">
+      <c r="E197" t="n">
+        <v>1861484</v>
+      </c>
+      <c r="F197" t="n">
+        <v>41801533</v>
+      </c>
+      <c r="G197" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sd.gif</t>
         </is>
@@ -5773,7 +6959,13 @@
           <t>Stockholm</t>
         </is>
       </c>
-      <c r="E198" t="inlineStr">
+      <c r="E198" t="n">
+        <v>449964</v>
+      </c>
+      <c r="F198" t="n">
+        <v>10183175</v>
+      </c>
+      <c r="G198" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/se.gif</t>
         </is>
@@ -5800,7 +6992,13 @@
           <t>Singapore</t>
         </is>
       </c>
-      <c r="E199" t="inlineStr">
+      <c r="E199" t="n">
+        <v>692.7</v>
+      </c>
+      <c r="F199" t="n">
+        <v>5638676</v>
+      </c>
+      <c r="G199" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sg.gif</t>
         </is>
@@ -5827,7 +7025,13 @@
           <t>Jamestown</t>
         </is>
       </c>
-      <c r="E200" t="inlineStr">
+      <c r="E200" t="n">
+        <v>410</v>
+      </c>
+      <c r="F200" t="n">
+        <v>7460</v>
+      </c>
+      <c r="G200" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sh.gif</t>
         </is>
@@ -5854,7 +7058,13 @@
           <t>Ljubljana</t>
         </is>
       </c>
-      <c r="E201" t="inlineStr">
+      <c r="E201" t="n">
+        <v>20273</v>
+      </c>
+      <c r="F201" t="n">
+        <v>2067372</v>
+      </c>
+      <c r="G201" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/si.gif</t>
         </is>
@@ -5881,7 +7091,13 @@
           <t>Longyearbyen</t>
         </is>
       </c>
-      <c r="E202" t="inlineStr">
+      <c r="E202" t="n">
+        <v>62049</v>
+      </c>
+      <c r="F202" t="n">
+        <v>2550</v>
+      </c>
+      <c r="G202" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sj.gif</t>
         </is>
@@ -5908,7 +7124,13 @@
           <t>Bratislava</t>
         </is>
       </c>
-      <c r="E203" t="inlineStr">
+      <c r="E203" t="n">
+        <v>48845</v>
+      </c>
+      <c r="F203" t="n">
+        <v>5447011</v>
+      </c>
+      <c r="G203" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sk.gif</t>
         </is>
@@ -5935,7 +7157,13 @@
           <t>Freetown</t>
         </is>
       </c>
-      <c r="E204" t="inlineStr">
+      <c r="E204" t="n">
+        <v>71740</v>
+      </c>
+      <c r="F204" t="n">
+        <v>7650154</v>
+      </c>
+      <c r="G204" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sl.gif</t>
         </is>
@@ -5962,7 +7190,13 @@
           <t>San Marino</t>
         </is>
       </c>
-      <c r="E205" t="inlineStr">
+      <c r="E205" t="n">
+        <v>61.2</v>
+      </c>
+      <c r="F205" t="n">
+        <v>33785</v>
+      </c>
+      <c r="G205" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sm.gif</t>
         </is>
@@ -5989,7 +7223,13 @@
           <t>Dakar</t>
         </is>
       </c>
-      <c r="E206" t="inlineStr">
+      <c r="E206" t="n">
+        <v>196190</v>
+      </c>
+      <c r="F206" t="n">
+        <v>15854360</v>
+      </c>
+      <c r="G206" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sn.gif</t>
         </is>
@@ -6016,7 +7256,13 @@
           <t>Mogadishu</t>
         </is>
       </c>
-      <c r="E207" t="inlineStr">
+      <c r="E207" t="n">
+        <v>637657</v>
+      </c>
+      <c r="F207" t="n">
+        <v>15008154</v>
+      </c>
+      <c r="G207" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/so.gif</t>
         </is>
@@ -6043,7 +7289,13 @@
           <t>Paramaribo</t>
         </is>
       </c>
-      <c r="E208" t="inlineStr">
+      <c r="E208" t="n">
+        <v>163270</v>
+      </c>
+      <c r="F208" t="n">
+        <v>575991</v>
+      </c>
+      <c r="G208" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sr.gif</t>
         </is>
@@ -6070,7 +7322,13 @@
           <t>Juba</t>
         </is>
       </c>
-      <c r="E209" t="inlineStr">
+      <c r="E209" t="n">
+        <v>644329</v>
+      </c>
+      <c r="F209" t="n">
+        <v>8260490</v>
+      </c>
+      <c r="G209" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ss.gif</t>
         </is>
@@ -6097,7 +7355,13 @@
           <t>Sao Tome</t>
         </is>
       </c>
-      <c r="E210" t="inlineStr">
+      <c r="E210" t="n">
+        <v>1001</v>
+      </c>
+      <c r="F210" t="n">
+        <v>197700</v>
+      </c>
+      <c r="G210" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/st.gif</t>
         </is>
@@ -6124,7 +7388,13 @@
           <t>San Salvador</t>
         </is>
       </c>
-      <c r="E211" t="inlineStr">
+      <c r="E211" t="n">
+        <v>21040</v>
+      </c>
+      <c r="F211" t="n">
+        <v>6420744</v>
+      </c>
+      <c r="G211" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sv.gif</t>
         </is>
@@ -6151,7 +7421,13 @@
           <t>Philipsburg</t>
         </is>
       </c>
-      <c r="E212" t="inlineStr">
+      <c r="E212" t="n">
+        <v>21</v>
+      </c>
+      <c r="F212" t="n">
+        <v>40654</v>
+      </c>
+      <c r="G212" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sx.gif</t>
         </is>
@@ -6178,7 +7454,13 @@
           <t>Damascus</t>
         </is>
       </c>
-      <c r="E213" t="inlineStr">
+      <c r="E213" t="n">
+        <v>185180</v>
+      </c>
+      <c r="F213" t="n">
+        <v>16906283</v>
+      </c>
+      <c r="G213" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sy.gif</t>
         </is>
@@ -6205,7 +7487,13 @@
           <t>Mbabane</t>
         </is>
       </c>
-      <c r="E214" t="inlineStr">
+      <c r="E214" t="n">
+        <v>17363</v>
+      </c>
+      <c r="F214" t="n">
+        <v>1136191</v>
+      </c>
+      <c r="G214" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/sz.gif</t>
         </is>
@@ -6232,7 +7520,13 @@
           <t>Cockburn Town</t>
         </is>
       </c>
-      <c r="E215" t="inlineStr">
+      <c r="E215" t="n">
+        <v>430</v>
+      </c>
+      <c r="F215" t="n">
+        <v>37665</v>
+      </c>
+      <c r="G215" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/tc.gif</t>
         </is>
@@ -6259,7 +7553,13 @@
           <t>N'Djamena</t>
         </is>
       </c>
-      <c r="E216" t="inlineStr">
+      <c r="E216" t="n">
+        <v>1284000</v>
+      </c>
+      <c r="F216" t="n">
+        <v>15477751</v>
+      </c>
+      <c r="G216" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/td.gif</t>
         </is>
@@ -6286,7 +7586,13 @@
           <t>Port-aux-Francais</t>
         </is>
       </c>
-      <c r="E217" t="inlineStr">
+      <c r="E217" t="n">
+        <v>7829</v>
+      </c>
+      <c r="F217" t="n">
+        <v>140</v>
+      </c>
+      <c r="G217" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/tf.gif</t>
         </is>
@@ -6313,7 +7619,13 @@
           <t>Lome</t>
         </is>
       </c>
-      <c r="E218" t="inlineStr">
+      <c r="E218" t="n">
+        <v>56785</v>
+      </c>
+      <c r="F218" t="n">
+        <v>7889094</v>
+      </c>
+      <c r="G218" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/tg.gif</t>
         </is>
@@ -6340,7 +7652,13 @@
           <t>Bangkok</t>
         </is>
       </c>
-      <c r="E219" t="inlineStr">
+      <c r="E219" t="n">
+        <v>514000</v>
+      </c>
+      <c r="F219" t="n">
+        <v>69428524</v>
+      </c>
+      <c r="G219" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/th.gif</t>
         </is>
@@ -6367,7 +7685,13 @@
           <t>Dushanbe</t>
         </is>
       </c>
-      <c r="E220" t="inlineStr">
+      <c r="E220" t="n">
+        <v>143100</v>
+      </c>
+      <c r="F220" t="n">
+        <v>9100837</v>
+      </c>
+      <c r="G220" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/tj.gif</t>
         </is>
@@ -6394,7 +7718,13 @@
           <t>Toquelau</t>
         </is>
       </c>
-      <c r="E221" t="inlineStr">
+      <c r="E221" t="n">
+        <v>10</v>
+      </c>
+      <c r="F221" t="n">
+        <v>1466</v>
+      </c>
+      <c r="G221" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/tk.gif</t>
         </is>
@@ -6421,7 +7751,13 @@
           <t>Dili</t>
         </is>
       </c>
-      <c r="E222" t="inlineStr">
+      <c r="E222" t="n">
+        <v>15007</v>
+      </c>
+      <c r="F222" t="n">
+        <v>1267972</v>
+      </c>
+      <c r="G222" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/tl.gif</t>
         </is>
@@ -6448,7 +7784,13 @@
           <t>Ashgabat</t>
         </is>
       </c>
-      <c r="E223" t="inlineStr">
+      <c r="E223" t="n">
+        <v>488100</v>
+      </c>
+      <c r="F223" t="n">
+        <v>5850908</v>
+      </c>
+      <c r="G223" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/tm.gif</t>
         </is>
@@ -6475,7 +7817,13 @@
           <t>Tunis</t>
         </is>
       </c>
-      <c r="E224" t="inlineStr">
+      <c r="E224" t="n">
+        <v>163610</v>
+      </c>
+      <c r="F224" t="n">
+        <v>11565204</v>
+      </c>
+      <c r="G224" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/tn.gif</t>
         </is>
@@ -6502,7 +7850,13 @@
           <t>Nuku'alofa</t>
         </is>
       </c>
-      <c r="E225" t="inlineStr">
+      <c r="E225" t="n">
+        <v>748</v>
+      </c>
+      <c r="F225" t="n">
+        <v>103197</v>
+      </c>
+      <c r="G225" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/to.gif</t>
         </is>
@@ -6529,7 +7883,13 @@
           <t>Ankara</t>
         </is>
       </c>
-      <c r="E226" t="inlineStr">
+      <c r="E226" t="n">
+        <v>780580</v>
+      </c>
+      <c r="F226" t="n">
+        <v>82319724</v>
+      </c>
+      <c r="G226" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/tr.gif</t>
         </is>
@@ -6556,7 +7916,13 @@
           <t>Port of Spain</t>
         </is>
       </c>
-      <c r="E227" t="inlineStr">
+      <c r="E227" t="n">
+        <v>5128</v>
+      </c>
+      <c r="F227" t="n">
+        <v>1389858</v>
+      </c>
+      <c r="G227" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/tt.gif</t>
         </is>
@@ -6583,7 +7949,13 @@
           <t>Funafuti</t>
         </is>
       </c>
-      <c r="E228" t="inlineStr">
+      <c r="E228" t="n">
+        <v>26</v>
+      </c>
+      <c r="F228" t="n">
+        <v>11508</v>
+      </c>
+      <c r="G228" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/tv.gif</t>
         </is>
@@ -6610,7 +7982,13 @@
           <t>Taipei</t>
         </is>
       </c>
-      <c r="E229" t="inlineStr">
+      <c r="E229" t="n">
+        <v>35980</v>
+      </c>
+      <c r="F229" t="n">
+        <v>23451837</v>
+      </c>
+      <c r="G229" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/tw.gif</t>
         </is>
@@ -6637,7 +8015,13 @@
           <t>Dodoma</t>
         </is>
       </c>
-      <c r="E230" t="inlineStr">
+      <c r="E230" t="n">
+        <v>945087</v>
+      </c>
+      <c r="F230" t="n">
+        <v>56318348</v>
+      </c>
+      <c r="G230" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/tz.gif</t>
         </is>
@@ -6664,7 +8048,13 @@
           <t>Kyiv</t>
         </is>
       </c>
-      <c r="E231" t="inlineStr">
+      <c r="E231" t="n">
+        <v>603700</v>
+      </c>
+      <c r="F231" t="n">
+        <v>44622516</v>
+      </c>
+      <c r="G231" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ua.gif</t>
         </is>
@@ -6691,7 +8081,13 @@
           <t>Kampala</t>
         </is>
       </c>
-      <c r="E232" t="inlineStr">
+      <c r="E232" t="n">
+        <v>236040</v>
+      </c>
+      <c r="F232" t="n">
+        <v>42723139</v>
+      </c>
+      <c r="G232" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ug.gif</t>
         </is>
@@ -6718,7 +8114,13 @@
           <t>Ilhas Distantes dos EUA</t>
         </is>
       </c>
-      <c r="E233" t="inlineStr">
+      <c r="E233" t="n">
+        <v>0</v>
+      </c>
+      <c r="F233" t="n">
+        <v>0</v>
+      </c>
+      <c r="G233" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/um.gif</t>
         </is>
@@ -6745,7 +8147,13 @@
           <t>Washington</t>
         </is>
       </c>
-      <c r="E234" t="inlineStr">
+      <c r="E234" t="n">
+        <v>9629091</v>
+      </c>
+      <c r="F234" t="n">
+        <v>327167434</v>
+      </c>
+      <c r="G234" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/us.gif</t>
         </is>
@@ -6772,7 +8180,13 @@
           <t>Montevideo</t>
         </is>
       </c>
-      <c r="E235" t="inlineStr">
+      <c r="E235" t="n">
+        <v>176220</v>
+      </c>
+      <c r="F235" t="n">
+        <v>3449299</v>
+      </c>
+      <c r="G235" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/uy.gif</t>
         </is>
@@ -6799,7 +8213,13 @@
           <t>Tashkent</t>
         </is>
       </c>
-      <c r="E236" t="inlineStr">
+      <c r="E236" t="n">
+        <v>447400</v>
+      </c>
+      <c r="F236" t="n">
+        <v>32955400</v>
+      </c>
+      <c r="G236" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/uz.gif</t>
         </is>
@@ -6826,7 +8246,13 @@
           <t>Vatican City</t>
         </is>
       </c>
-      <c r="E237" t="inlineStr">
+      <c r="E237" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F237" t="n">
+        <v>921</v>
+      </c>
+      <c r="G237" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/va.gif</t>
         </is>
@@ -6853,7 +8279,13 @@
           <t>Kingstown</t>
         </is>
       </c>
-      <c r="E238" t="inlineStr">
+      <c r="E238" t="n">
+        <v>389</v>
+      </c>
+      <c r="F238" t="n">
+        <v>110211</v>
+      </c>
+      <c r="G238" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/vc.gif</t>
         </is>
@@ -6880,7 +8312,13 @@
           <t>Caracas</t>
         </is>
       </c>
-      <c r="E239" t="inlineStr">
+      <c r="E239" t="n">
+        <v>912050</v>
+      </c>
+      <c r="F239" t="n">
+        <v>28870195</v>
+      </c>
+      <c r="G239" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ve.gif</t>
         </is>
@@ -6907,7 +8345,13 @@
           <t>Road Town</t>
         </is>
       </c>
-      <c r="E240" t="inlineStr">
+      <c r="E240" t="n">
+        <v>153</v>
+      </c>
+      <c r="F240" t="n">
+        <v>29802</v>
+      </c>
+      <c r="G240" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/vg.gif</t>
         </is>
@@ -6934,7 +8378,13 @@
           <t>Charlotte Amalie</t>
         </is>
       </c>
-      <c r="E241" t="inlineStr">
+      <c r="E241" t="n">
+        <v>352</v>
+      </c>
+      <c r="F241" t="n">
+        <v>106977</v>
+      </c>
+      <c r="G241" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/vi.gif</t>
         </is>
@@ -6961,7 +8411,13 @@
           <t>Hanoi</t>
         </is>
       </c>
-      <c r="E242" t="inlineStr">
+      <c r="E242" t="n">
+        <v>329560</v>
+      </c>
+      <c r="F242" t="n">
+        <v>95540395</v>
+      </c>
+      <c r="G242" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/vn.gif</t>
         </is>
@@ -6988,7 +8444,13 @@
           <t>Port Vila</t>
         </is>
       </c>
-      <c r="E243" t="inlineStr">
+      <c r="E243" t="n">
+        <v>12200</v>
+      </c>
+      <c r="F243" t="n">
+        <v>292680</v>
+      </c>
+      <c r="G243" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/vu.gif</t>
         </is>
@@ -7015,7 +8477,13 @@
           <t>Mata Utu</t>
         </is>
       </c>
-      <c r="E244" t="inlineStr">
+      <c r="E244" t="n">
+        <v>274</v>
+      </c>
+      <c r="F244" t="n">
+        <v>16025</v>
+      </c>
+      <c r="G244" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/wf.gif</t>
         </is>
@@ -7042,7 +8510,13 @@
           <t>Apia</t>
         </is>
       </c>
-      <c r="E245" t="inlineStr">
+      <c r="E245" t="n">
+        <v>2944</v>
+      </c>
+      <c r="F245" t="n">
+        <v>196130</v>
+      </c>
+      <c r="G245" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ws.gif</t>
         </is>
@@ -7069,7 +8543,13 @@
           <t>Pristina</t>
         </is>
       </c>
-      <c r="E246" t="inlineStr">
+      <c r="E246" t="n">
+        <v>10908</v>
+      </c>
+      <c r="F246" t="n">
+        <v>1845300</v>
+      </c>
+      <c r="G246" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/xk.gif</t>
         </is>
@@ -7096,7 +8576,13 @@
           <t>Sanaa</t>
         </is>
       </c>
-      <c r="E247" t="inlineStr">
+      <c r="E247" t="n">
+        <v>527970</v>
+      </c>
+      <c r="F247" t="n">
+        <v>28498687</v>
+      </c>
+      <c r="G247" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/ye.gif</t>
         </is>
@@ -7123,7 +8609,13 @@
           <t>Mamoudzou</t>
         </is>
       </c>
-      <c r="E248" t="inlineStr">
+      <c r="E248" t="n">
+        <v>374</v>
+      </c>
+      <c r="F248" t="n">
+        <v>279471</v>
+      </c>
+      <c r="G248" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/yt.gif</t>
         </is>
@@ -7150,7 +8642,13 @@
           <t>Pretoria</t>
         </is>
       </c>
-      <c r="E249" t="inlineStr">
+      <c r="E249" t="n">
+        <v>1219912</v>
+      </c>
+      <c r="F249" t="n">
+        <v>57779622</v>
+      </c>
+      <c r="G249" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/za.gif</t>
         </is>
@@ -7177,7 +8675,13 @@
           <t>Lusaka</t>
         </is>
       </c>
-      <c r="E250" t="inlineStr">
+      <c r="E250" t="n">
+        <v>752614</v>
+      </c>
+      <c r="F250" t="n">
+        <v>17351822</v>
+      </c>
+      <c r="G250" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/zm.gif</t>
         </is>
@@ -7204,7 +8708,13 @@
           <t>Harare</t>
         </is>
       </c>
-      <c r="E251" t="inlineStr">
+      <c r="E251" t="n">
+        <v>390580</v>
+      </c>
+      <c r="F251" t="n">
+        <v>14439018</v>
+      </c>
+      <c r="G251" t="inlineStr">
         <is>
           <t>http://www.geonames.org/flags/x/zw.gif</t>
         </is>

</xml_diff>